<commit_message>
Update correction() method data loading and example data
</commit_message>
<xml_diff>
--- a/exampledata.xlsx
+++ b/exampledata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamp\PycharmProjects\Miscal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF451DC8-2495-48EA-B81A-AD5AA99B330F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8E1FEA5-278F-4D3F-A3C5-31B779EAFDA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="0" windowWidth="24420" windowHeight="11790" xr2:uid="{E07B14D5-2B45-408E-8D02-4ECED7EB5B15}"/>
   </bookViews>
@@ -381,15 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E90D1C-1530-4A1E-B577-1A9B7C4B4017}">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I80"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>0.24062434999999999</v>
       </c>
@@ -397,28 +397,22 @@
         <v>4.2848858999999999</v>
       </c>
       <c r="C1" s="1">
-        <v>-1.1420774999999999E-2</v>
+        <v>200</v>
       </c>
       <c r="D1" s="1">
-        <v>198.60243</v>
+        <v>0.23531915</v>
       </c>
       <c r="E1" s="1">
-        <v>200</v>
+        <v>0.24641184999999999</v>
       </c>
       <c r="F1" s="1">
-        <v>0.23531915</v>
+        <v>3.2608624000000002</v>
       </c>
       <c r="G1" s="1">
-        <v>0.24641184999999999</v>
-      </c>
-      <c r="H1" s="1">
-        <v>3.2608624000000002</v>
-      </c>
-      <c r="I1" s="1">
         <v>2.8067548000000002</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.26731893000000001</v>
       </c>
@@ -426,28 +420,22 @@
         <v>4.2402863999999996</v>
       </c>
       <c r="C2" s="1">
-        <v>-1.4954535999999999E-2</v>
+        <v>206.32911999999999</v>
       </c>
       <c r="D2" s="1">
-        <v>204.7765</v>
+        <v>0.27391008</v>
       </c>
       <c r="E2" s="1">
-        <v>206.32911999999999</v>
+        <v>0.26012858999999999</v>
       </c>
       <c r="F2" s="1">
-        <v>0.27391008</v>
+        <v>3.2632945000000002</v>
       </c>
       <c r="G2" s="1">
-        <v>0.26012858999999999</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3.2632945000000002</v>
-      </c>
-      <c r="I2" s="1">
         <v>2.8428035</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.29273883000000001</v>
       </c>
@@ -455,28 +443,22 @@
         <v>4.1711197000000002</v>
       </c>
       <c r="C3" s="1">
-        <v>-1.2145889E-2</v>
+        <v>212.65823</v>
       </c>
       <c r="D3" s="1">
-        <v>210.95797999999999</v>
+        <v>0.27489063000000002</v>
       </c>
       <c r="E3" s="1">
-        <v>212.65823</v>
+        <v>0.31220957999999999</v>
       </c>
       <c r="F3" s="1">
-        <v>0.27489063000000002</v>
+        <v>3.1837580000000001</v>
       </c>
       <c r="G3" s="1">
-        <v>0.31220957999999999</v>
-      </c>
-      <c r="H3" s="1">
-        <v>3.1837580000000001</v>
-      </c>
-      <c r="I3" s="1">
         <v>2.7453232000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.32975039</v>
       </c>
@@ -484,28 +466,22 @@
         <v>4.232996</v>
       </c>
       <c r="C4" s="1">
-        <v>-3.5347007E-2</v>
+        <v>218.98733999999999</v>
       </c>
       <c r="D4" s="1">
-        <v>217.07212999999999</v>
+        <v>0.35592371</v>
       </c>
       <c r="E4" s="1">
-        <v>218.98733999999999</v>
+        <v>0.30119764999999998</v>
       </c>
       <c r="F4" s="1">
-        <v>0.35592371</v>
+        <v>3.2255007999999998</v>
       </c>
       <c r="G4" s="1">
-        <v>0.30119764999999998</v>
-      </c>
-      <c r="H4" s="1">
-        <v>3.2255007999999998</v>
-      </c>
-      <c r="I4" s="1">
         <v>2.7726609999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.31531285999999997</v>
       </c>
@@ -513,28 +489,22 @@
         <v>4.2638458999999997</v>
       </c>
       <c r="C5" s="1">
-        <v>-6.2424305000000004E-4</v>
+        <v>225.31645</v>
       </c>
       <c r="D5" s="1">
-        <v>223.48509000000001</v>
+        <v>0.27898096999999999</v>
       </c>
       <c r="E5" s="1">
-        <v>225.31645</v>
+        <v>0.35494763000000001</v>
       </c>
       <c r="F5" s="1">
-        <v>0.27898096999999999</v>
+        <v>3.2302529999999998</v>
       </c>
       <c r="G5" s="1">
-        <v>0.35494763000000001</v>
-      </c>
-      <c r="H5" s="1">
-        <v>3.2302529999999998</v>
-      </c>
-      <c r="I5" s="1">
         <v>2.8554192</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.37569701999999999</v>
       </c>
@@ -542,28 +512,22 @@
         <v>4.2456369</v>
       </c>
       <c r="C6" s="1">
-        <v>-1.2075127999999999E-2</v>
+        <v>231.64556999999999</v>
       </c>
       <c r="D6" s="1">
-        <v>229.46349000000001</v>
+        <v>0.37519711</v>
       </c>
       <c r="E6" s="1">
-        <v>231.64556999999999</v>
+        <v>0.37624236999999999</v>
       </c>
       <c r="F6" s="1">
-        <v>0.37519711</v>
+        <v>3.1806673999999999</v>
       </c>
       <c r="G6" s="1">
-        <v>0.37624236999999999</v>
-      </c>
-      <c r="H6" s="1">
-        <v>3.1806673999999999</v>
-      </c>
-      <c r="I6" s="1">
         <v>2.8336712999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.39028015999999999</v>
       </c>
@@ -571,28 +535,22 @@
         <v>4.1550918000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>-8.4297721999999995E-3</v>
+        <v>237.97469000000001</v>
       </c>
       <c r="D7" s="1">
-        <v>235.7079</v>
+        <v>0.40185976000000001</v>
       </c>
       <c r="E7" s="1">
-        <v>237.97469000000001</v>
+        <v>0.37764785000000001</v>
       </c>
       <c r="F7" s="1">
-        <v>0.40185976000000001</v>
+        <v>3.1140317999999998</v>
       </c>
       <c r="G7" s="1">
-        <v>0.37764785000000001</v>
-      </c>
-      <c r="H7" s="1">
-        <v>3.1140317999999998</v>
-      </c>
-      <c r="I7" s="1">
         <v>2.7353589999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.42093560000000002</v>
       </c>
@@ -600,28 +558,22 @@
         <v>4.1274476</v>
       </c>
       <c r="C8" s="1">
-        <v>3.8112286000000002E-2</v>
+        <v>244.3038</v>
       </c>
       <c r="D8" s="1">
-        <v>241.85896</v>
+        <v>0.41930964999999998</v>
       </c>
       <c r="E8" s="1">
-        <v>244.3038</v>
+        <v>0.42270934999999998</v>
       </c>
       <c r="F8" s="1">
-        <v>0.41930964999999998</v>
+        <v>3.1273021999999999</v>
       </c>
       <c r="G8" s="1">
-        <v>0.42270934999999998</v>
-      </c>
-      <c r="H8" s="1">
-        <v>3.1273021999999999</v>
-      </c>
-      <c r="I8" s="1">
         <v>2.7743308999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.47491973999999998</v>
       </c>
@@ -629,28 +581,22 @@
         <v>4.2186994999999996</v>
       </c>
       <c r="C9" s="1">
-        <v>9.8124370000000002E-3</v>
+        <v>250.63290000000001</v>
       </c>
       <c r="D9" s="1">
-        <v>247.87454</v>
+        <v>0.47372690000000001</v>
       </c>
       <c r="E9" s="1">
-        <v>250.63290000000001</v>
+        <v>0.47622101999999999</v>
       </c>
       <c r="F9" s="1">
-        <v>0.47372690000000001</v>
+        <v>3.1705093</v>
       </c>
       <c r="G9" s="1">
-        <v>0.47622101999999999</v>
-      </c>
-      <c r="H9" s="1">
-        <v>3.1705093</v>
-      </c>
-      <c r="I9" s="1">
         <v>2.8856435</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.49571409999999999</v>
       </c>
@@ -658,28 +604,22 @@
         <v>4.0897421999999999</v>
       </c>
       <c r="C10" s="1">
-        <v>2.0179953E-2</v>
+        <v>256.96204</v>
       </c>
       <c r="D10" s="1">
-        <v>254.08287000000001</v>
+        <v>0.51019203999999996</v>
       </c>
       <c r="E10" s="1">
-        <v>256.96204</v>
+        <v>0.47992000000000001</v>
       </c>
       <c r="F10" s="1">
-        <v>0.51019203999999996</v>
+        <v>3.1737747000000001</v>
       </c>
       <c r="G10" s="1">
-        <v>0.47992000000000001</v>
-      </c>
-      <c r="H10" s="1">
-        <v>3.1737747000000001</v>
-      </c>
-      <c r="I10" s="1">
         <v>2.7651349999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.58271342999999998</v>
       </c>
@@ -687,28 +627,22 @@
         <v>4.0699100000000001</v>
       </c>
       <c r="C11" s="1">
-        <v>1.6952841999999999E-2</v>
+        <v>263.29113999999998</v>
       </c>
       <c r="D11" s="1">
-        <v>259.90670999999998</v>
+        <v>0.55398428</v>
       </c>
       <c r="E11" s="1">
-        <v>263.29113999999998</v>
+        <v>0.61405438000000001</v>
       </c>
       <c r="F11" s="1">
-        <v>0.55398428</v>
+        <v>3.1786232000000001</v>
       </c>
       <c r="G11" s="1">
-        <v>0.61405438000000001</v>
-      </c>
-      <c r="H11" s="1">
-        <v>3.1786232000000001</v>
-      </c>
-      <c r="I11" s="1">
         <v>2.7636666000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.67454225000000001</v>
       </c>
@@ -716,28 +650,22 @@
         <v>4.1514024999999997</v>
       </c>
       <c r="C12" s="1">
-        <v>-4.3413426999999997E-2</v>
+        <v>269.62024000000002</v>
       </c>
       <c r="D12" s="1">
-        <v>265.70245</v>
+        <v>0.69212878</v>
       </c>
       <c r="E12" s="1">
-        <v>269.62024000000002</v>
+        <v>0.65535688000000003</v>
       </c>
       <c r="F12" s="1">
-        <v>0.69212878</v>
+        <v>3.1306474</v>
       </c>
       <c r="G12" s="1">
-        <v>0.65535688000000003</v>
-      </c>
-      <c r="H12" s="1">
-        <v>3.1306474</v>
-      </c>
-      <c r="I12" s="1">
         <v>2.8343216999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.72365217999999998</v>
       </c>
@@ -745,28 +673,22 @@
         <v>4.1093006000000001</v>
       </c>
       <c r="C13" s="1">
-        <v>2.8281197000000001E-2</v>
+        <v>275.94936999999999</v>
       </c>
       <c r="D13" s="1">
-        <v>271.74633999999998</v>
+        <v>0.74757266</v>
       </c>
       <c r="E13" s="1">
-        <v>275.94936999999999</v>
+        <v>0.69755703000000002</v>
       </c>
       <c r="F13" s="1">
-        <v>0.74757266</v>
+        <v>3.1120000000000001</v>
       </c>
       <c r="G13" s="1">
-        <v>0.69755703000000002</v>
-      </c>
-      <c r="H13" s="1">
-        <v>3.1120000000000001</v>
-      </c>
-      <c r="I13" s="1">
         <v>2.7945137</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.84144001999999996</v>
       </c>
@@ -774,28 +696,22 @@
         <v>4.0303750000000003</v>
       </c>
       <c r="C14" s="1">
-        <v>-1.374324E-2</v>
+        <v>282.27847000000003</v>
       </c>
       <c r="D14" s="1">
-        <v>277.39132999999998</v>
+        <v>0.88159715999999999</v>
       </c>
       <c r="E14" s="1">
-        <v>282.27847000000003</v>
+        <v>0.79763222</v>
       </c>
       <c r="F14" s="1">
-        <v>0.88159715999999999</v>
+        <v>3.0617321</v>
       </c>
       <c r="G14" s="1">
-        <v>0.79763222</v>
-      </c>
-      <c r="H14" s="1">
-        <v>3.0617321</v>
-      </c>
-      <c r="I14" s="1">
         <v>2.7204191999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.94840252000000003</v>
       </c>
@@ -803,28 +719,22 @@
         <v>4.0127496999999996</v>
       </c>
       <c r="C15" s="1">
-        <v>9.7281665000000003E-2</v>
+        <v>288.60759999999999</v>
       </c>
       <c r="D15" s="1">
-        <v>283.09917999999999</v>
+        <v>0.93285518999999995</v>
       </c>
       <c r="E15" s="1">
-        <v>288.60759999999999</v>
+        <v>0.96536319999999998</v>
       </c>
       <c r="F15" s="1">
-        <v>0.93285518999999995</v>
+        <v>3.1107999999999998</v>
       </c>
       <c r="G15" s="1">
-        <v>0.96536319999999998</v>
-      </c>
-      <c r="H15" s="1">
-        <v>3.1107999999999998</v>
-      </c>
-      <c r="I15" s="1">
         <v>2.7778160999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1.0680791999999999</v>
       </c>
@@ -832,28 +742,22 @@
         <v>3.9519467000000001</v>
       </c>
       <c r="C16" s="1">
-        <v>4.3755449000000002E-2</v>
+        <v>294.93671000000001</v>
       </c>
       <c r="D16" s="1">
-        <v>288.73322000000002</v>
+        <v>1.070899</v>
       </c>
       <c r="E16" s="1">
-        <v>294.93671000000001</v>
+        <v>1.0650029999999999</v>
       </c>
       <c r="F16" s="1">
-        <v>1.070899</v>
+        <v>3.0534124</v>
       </c>
       <c r="G16" s="1">
-        <v>1.0650029999999999</v>
-      </c>
-      <c r="H16" s="1">
-        <v>3.0534124</v>
-      </c>
-      <c r="I16" s="1">
         <v>2.7015090000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1.2143164</v>
       </c>
@@ -861,28 +765,22 @@
         <v>3.8222619999999998</v>
       </c>
       <c r="C17" s="1">
-        <v>2.5747642000000001E-2</v>
+        <v>301.26580999999999</v>
       </c>
       <c r="D17" s="1">
-        <v>294.21298000000002</v>
+        <v>1.2253064</v>
       </c>
       <c r="E17" s="1">
-        <v>301.26580999999999</v>
+        <v>1.2023273000000001</v>
       </c>
       <c r="F17" s="1">
-        <v>1.2253064</v>
+        <v>3.0747339999999999</v>
       </c>
       <c r="G17" s="1">
-        <v>1.2023273000000001</v>
-      </c>
-      <c r="H17" s="1">
-        <v>3.0747339999999999</v>
-      </c>
-      <c r="I17" s="1">
         <v>2.6264485999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1.4257586</v>
       </c>
@@ -890,28 +788,22 @@
         <v>3.7797405999999998</v>
       </c>
       <c r="C18" s="1">
-        <v>4.3514672999999997E-2</v>
+        <v>307.59494000000001</v>
       </c>
       <c r="D18" s="1">
-        <v>299.31403</v>
+        <v>1.4279455999999999</v>
       </c>
       <c r="E18" s="1">
-        <v>307.59494000000001</v>
+        <v>1.4233726</v>
       </c>
       <c r="F18" s="1">
-        <v>1.4279455999999999</v>
+        <v>3.1078217000000001</v>
       </c>
       <c r="G18" s="1">
-        <v>1.4233726</v>
-      </c>
-      <c r="H18" s="1">
-        <v>3.1078217000000001</v>
-      </c>
-      <c r="I18" s="1">
         <v>2.6977768000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1.6664855000000001</v>
       </c>
@@ -919,28 +811,22 @@
         <v>3.6785304999999999</v>
       </c>
       <c r="C19" s="1">
-        <v>0.10226879</v>
+        <v>313.92403999999999</v>
       </c>
       <c r="D19" s="1">
-        <v>304.24495999999999</v>
+        <v>1.6885695000000001</v>
       </c>
       <c r="E19" s="1">
-        <v>313.92403999999999</v>
+        <v>1.6423938</v>
       </c>
       <c r="F19" s="1">
-        <v>1.6885695000000001</v>
+        <v>3.0047839000000001</v>
       </c>
       <c r="G19" s="1">
-        <v>1.6423938</v>
-      </c>
-      <c r="H19" s="1">
-        <v>3.0047839000000001</v>
-      </c>
-      <c r="I19" s="1">
         <v>2.6007562000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1.9289414</v>
       </c>
@@ -948,28 +834,22 @@
         <v>3.4636252000000001</v>
       </c>
       <c r="C20" s="1">
-        <v>0.10545573</v>
+        <v>320.25317000000001</v>
       </c>
       <c r="D20" s="1">
-        <v>309.04971</v>
+        <v>1.9473168000000001</v>
       </c>
       <c r="E20" s="1">
-        <v>320.25317000000001</v>
+        <v>1.9088955000000001</v>
       </c>
       <c r="F20" s="1">
-        <v>1.9473168000000001</v>
+        <v>2.9340236000000002</v>
       </c>
       <c r="G20" s="1">
-        <v>1.9088955000000001</v>
-      </c>
-      <c r="H20" s="1">
-        <v>2.9340236000000002</v>
-      </c>
-      <c r="I20" s="1">
         <v>2.6141361999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2.2535443000000002</v>
       </c>
@@ -977,28 +857,22 @@
         <v>3.3869874000000002</v>
       </c>
       <c r="C21" s="1">
-        <v>0.12509902000000001</v>
+        <v>326.58228000000003</v>
       </c>
       <c r="D21" s="1">
-        <v>313.49349999999998</v>
+        <v>2.3363824000000002</v>
       </c>
       <c r="E21" s="1">
-        <v>326.58228000000003</v>
+        <v>2.1631756000000002</v>
       </c>
       <c r="F21" s="1">
-        <v>2.3363824000000002</v>
+        <v>2.8928153999999999</v>
       </c>
       <c r="G21" s="1">
-        <v>2.1631756000000002</v>
-      </c>
-      <c r="H21" s="1">
-        <v>2.8928153999999999</v>
-      </c>
-      <c r="I21" s="1">
         <v>2.6496765999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2.6196226999999999</v>
       </c>
@@ -1006,28 +880,22 @@
         <v>3.1846993000000001</v>
       </c>
       <c r="C22" s="1">
-        <v>0.11393884</v>
+        <v>332.91140999999999</v>
       </c>
       <c r="D22" s="1">
-        <v>317.69641000000001</v>
+        <v>2.6486287000000002</v>
       </c>
       <c r="E22" s="1">
-        <v>332.91140999999999</v>
+        <v>2.5879796000000002</v>
       </c>
       <c r="F22" s="1">
-        <v>2.6486287000000002</v>
+        <v>2.8413667999999999</v>
       </c>
       <c r="G22" s="1">
-        <v>2.5879796000000002</v>
-      </c>
-      <c r="H22" s="1">
-        <v>2.8413667999999999</v>
-      </c>
-      <c r="I22" s="1">
         <v>2.545372</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3.0481622000000002</v>
       </c>
@@ -1035,28 +903,22 @@
         <v>3.0922092999999999</v>
       </c>
       <c r="C23" s="1">
-        <v>0.11448216</v>
+        <v>339.24050999999997</v>
       </c>
       <c r="D23" s="1">
-        <v>321.53653000000003</v>
+        <v>3.0580001000000001</v>
       </c>
       <c r="E23" s="1">
-        <v>339.24050999999997</v>
+        <v>3.0374298</v>
       </c>
       <c r="F23" s="1">
-        <v>3.0580001000000001</v>
+        <v>2.8231250999999999</v>
       </c>
       <c r="G23" s="1">
-        <v>3.0374298</v>
-      </c>
-      <c r="H23" s="1">
-        <v>2.8231250999999999</v>
-      </c>
-      <c r="I23" s="1">
         <v>2.4755478000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>3.4995861000000001</v>
       </c>
@@ -1064,28 +926,22 @@
         <v>2.8199584</v>
       </c>
       <c r="C24" s="1">
-        <v>0.16936539</v>
+        <v>345.56961000000001</v>
       </c>
       <c r="D24" s="1">
-        <v>325.24374</v>
+        <v>3.5559707</v>
       </c>
       <c r="E24" s="1">
-        <v>345.56961000000001</v>
+        <v>3.4380760000000001</v>
       </c>
       <c r="F24" s="1">
-        <v>3.5559707</v>
+        <v>2.6981801999999999</v>
       </c>
       <c r="G24" s="1">
-        <v>3.4380760000000001</v>
-      </c>
-      <c r="H24" s="1">
-        <v>2.6981801999999999</v>
-      </c>
-      <c r="I24" s="1">
         <v>2.4032578</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4.0075396999999997</v>
       </c>
@@ -1093,28 +949,22 @@
         <v>2.7030091000000001</v>
       </c>
       <c r="C25" s="1">
-        <v>0.15758282000000001</v>
+        <v>351.89873999999998</v>
       </c>
       <c r="D25" s="1">
-        <v>328.62261999999998</v>
+        <v>4.0763559000000003</v>
       </c>
       <c r="E25" s="1">
-        <v>351.89873999999998</v>
+        <v>3.9324682000000002</v>
       </c>
       <c r="F25" s="1">
-        <v>4.0763559000000003</v>
+        <v>2.7299761999999999</v>
       </c>
       <c r="G25" s="1">
-        <v>3.9324682000000002</v>
-      </c>
-      <c r="H25" s="1">
-        <v>2.7299761999999999</v>
-      </c>
-      <c r="I25" s="1">
         <v>2.3933651</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>4.5655292999999997</v>
       </c>
@@ -1122,28 +972,22 @@
         <v>2.5227200999999999</v>
       </c>
       <c r="C26" s="1">
-        <v>0.15126297999999999</v>
+        <v>358.22784000000001</v>
       </c>
       <c r="D26" s="1">
-        <v>331.71087999999997</v>
+        <v>4.6365103999999997</v>
       </c>
       <c r="E26" s="1">
-        <v>358.22784000000001</v>
+        <v>4.4880947999999998</v>
       </c>
       <c r="F26" s="1">
-        <v>4.6365103999999997</v>
+        <v>2.5968396999999999</v>
       </c>
       <c r="G26" s="1">
-        <v>4.4880947999999998</v>
-      </c>
-      <c r="H26" s="1">
-        <v>2.5968396999999999</v>
-      </c>
-      <c r="I26" s="1">
         <v>2.3298416</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>5.1658758999999996</v>
       </c>
@@ -1151,28 +995,22 @@
         <v>2.3708067000000002</v>
       </c>
       <c r="C27" s="1">
-        <v>0.1915586</v>
+        <v>364.55698000000001</v>
       </c>
       <c r="D27" s="1">
-        <v>334.55313000000001</v>
+        <v>5.2619758000000001</v>
       </c>
       <c r="E27" s="1">
-        <v>364.55698000000001</v>
+        <v>5.0610404000000004</v>
       </c>
       <c r="F27" s="1">
-        <v>5.2619758000000001</v>
+        <v>2.6077487000000001</v>
       </c>
       <c r="G27" s="1">
-        <v>5.0610404000000004</v>
-      </c>
-      <c r="H27" s="1">
-        <v>2.6077487000000001</v>
-      </c>
-      <c r="I27" s="1">
         <v>2.3120883000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>5.7864617999999997</v>
       </c>
@@ -1180,28 +1018,22 @@
         <v>2.1986246</v>
       </c>
       <c r="C28" s="1">
-        <v>0.18060105000000001</v>
+        <v>370.88607999999999</v>
       </c>
       <c r="D28" s="1">
-        <v>337.27782999999999</v>
+        <v>5.8985105000000004</v>
       </c>
       <c r="E28" s="1">
-        <v>370.88607999999999</v>
+        <v>5.6642270000000003</v>
       </c>
       <c r="F28" s="1">
-        <v>5.8985105000000004</v>
+        <v>2.5371008000000002</v>
       </c>
       <c r="G28" s="1">
-        <v>5.6642270000000003</v>
-      </c>
-      <c r="H28" s="1">
-        <v>2.5371008000000002</v>
-      </c>
-      <c r="I28" s="1">
         <v>2.2716959000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>6.4517955999999996</v>
       </c>
@@ -1209,28 +1041,22 @@
         <v>2.1092787</v>
       </c>
       <c r="C29" s="1">
-        <v>0.13333210000000001</v>
+        <v>377.21517999999998</v>
       </c>
       <c r="D29" s="1">
-        <v>339.74265000000003</v>
+        <v>6.5478101000000004</v>
       </c>
       <c r="E29" s="1">
-        <v>377.21517999999998</v>
+        <v>6.3470521</v>
       </c>
       <c r="F29" s="1">
-        <v>6.5478101000000004</v>
+        <v>2.5565782000000001</v>
       </c>
       <c r="G29" s="1">
-        <v>6.3470521</v>
-      </c>
-      <c r="H29" s="1">
-        <v>2.5565782000000001</v>
-      </c>
-      <c r="I29" s="1">
         <v>2.2401559</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>7.1288285</v>
       </c>
@@ -1238,28 +1064,22 @@
         <v>1.9608612000000001</v>
       </c>
       <c r="C30" s="1">
-        <v>0.20341366999999999</v>
+        <v>383.54431</v>
       </c>
       <c r="D30" s="1">
-        <v>342.1395</v>
+        <v>7.2172909000000001</v>
       </c>
       <c r="E30" s="1">
-        <v>383.54431</v>
+        <v>7.0323243</v>
       </c>
       <c r="F30" s="1">
-        <v>7.2172909000000001</v>
+        <v>2.4755557000000001</v>
       </c>
       <c r="G30" s="1">
-        <v>7.0323243</v>
-      </c>
-      <c r="H30" s="1">
-        <v>2.4755557000000001</v>
-      </c>
-      <c r="I30" s="1">
         <v>2.2165039000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>7.8239030999999999</v>
       </c>
@@ -1267,28 +1087,22 @@
         <v>1.890023</v>
       </c>
       <c r="C31" s="1">
-        <v>0.23021438999999999</v>
+        <v>389.87340999999998</v>
       </c>
       <c r="D31" s="1">
-        <v>344.43155000000002</v>
+        <v>7.9154286000000003</v>
       </c>
       <c r="E31" s="1">
-        <v>389.87340999999998</v>
+        <v>7.7240567000000002</v>
       </c>
       <c r="F31" s="1">
-        <v>7.9154286000000003</v>
+        <v>2.4676056000000002</v>
       </c>
       <c r="G31" s="1">
-        <v>7.7240567000000002</v>
-      </c>
-      <c r="H31" s="1">
-        <v>2.4676056000000002</v>
-      </c>
-      <c r="I31" s="1">
         <v>2.2143389999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>8.5446404999999999</v>
       </c>
@@ -1296,28 +1110,22 @@
         <v>1.7583016</v>
       </c>
       <c r="C32" s="1">
-        <v>0.18965675000000001</v>
+        <v>396.20254999999997</v>
       </c>
       <c r="D32" s="1">
-        <v>346.57454999999999</v>
+        <v>8.6733779999999996</v>
       </c>
       <c r="E32" s="1">
-        <v>396.20254999999997</v>
+        <v>8.4041996000000001</v>
       </c>
       <c r="F32" s="1">
-        <v>8.6733779999999996</v>
+        <v>2.4674056000000002</v>
       </c>
       <c r="G32" s="1">
-        <v>8.4041996000000001</v>
-      </c>
-      <c r="H32" s="1">
-        <v>2.4674056000000002</v>
-      </c>
-      <c r="I32" s="1">
         <v>2.2009563000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>9.2855921000000006</v>
       </c>
@@ -1325,28 +1133,22 @@
         <v>1.6632142000000001</v>
       </c>
       <c r="C33" s="1">
-        <v>0.22690888000000001</v>
+        <v>402.53165000000001</v>
       </c>
       <c r="D33" s="1">
-        <v>348.60019</v>
+        <v>9.4387559999999997</v>
       </c>
       <c r="E33" s="1">
-        <v>402.53165000000001</v>
+        <v>9.1185054999999995</v>
       </c>
       <c r="F33" s="1">
-        <v>9.4387559999999997</v>
+        <v>2.4502673000000001</v>
       </c>
       <c r="G33" s="1">
-        <v>9.1185054999999995</v>
-      </c>
-      <c r="H33" s="1">
-        <v>2.4502673000000001</v>
-      </c>
-      <c r="I33" s="1">
         <v>2.1564112</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>10.042063000000001</v>
       </c>
@@ -1354,28 +1156,22 @@
         <v>1.5774918</v>
       </c>
       <c r="C34" s="1">
-        <v>0.14890149</v>
+        <v>408.86075</v>
       </c>
       <c r="D34" s="1">
-        <v>350.53564</v>
+        <v>10.187586</v>
       </c>
       <c r="E34" s="1">
-        <v>408.86075</v>
+        <v>9.8833093999999999</v>
       </c>
       <c r="F34" s="1">
-        <v>10.187586</v>
+        <v>2.4213005999999999</v>
       </c>
       <c r="G34" s="1">
-        <v>9.8833093999999999</v>
-      </c>
-      <c r="H34" s="1">
-        <v>2.4213005999999999</v>
-      </c>
-      <c r="I34" s="1">
         <v>2.1347046000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>10.803255999999999</v>
       </c>
@@ -1383,28 +1179,22 @@
         <v>1.5092093</v>
       </c>
       <c r="C35" s="1">
-        <v>0.19907610000000001</v>
+        <v>415.18988000000002</v>
       </c>
       <c r="D35" s="1">
-        <v>352.44369999999998</v>
+        <v>10.946812</v>
       </c>
       <c r="E35" s="1">
-        <v>415.18988000000002</v>
+        <v>10.646649</v>
       </c>
       <c r="F35" s="1">
-        <v>10.946812</v>
+        <v>2.3983843</v>
       </c>
       <c r="G35" s="1">
-        <v>10.646649</v>
-      </c>
-      <c r="H35" s="1">
-        <v>2.3983843</v>
-      </c>
-      <c r="I35" s="1">
         <v>2.1623755</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>11.574572</v>
       </c>
@@ -1412,28 +1202,22 @@
         <v>1.4618053</v>
       </c>
       <c r="C36" s="1">
-        <v>0.19151620999999999</v>
+        <v>421.51898</v>
       </c>
       <c r="D36" s="1">
-        <v>354.29293999999999</v>
+        <v>11.767198</v>
       </c>
       <c r="E36" s="1">
-        <v>421.51898</v>
+        <v>11.364435</v>
       </c>
       <c r="F36" s="1">
-        <v>11.767198</v>
+        <v>2.4149181999999998</v>
       </c>
       <c r="G36" s="1">
-        <v>11.364435</v>
-      </c>
-      <c r="H36" s="1">
-        <v>2.4149181999999998</v>
-      </c>
-      <c r="I36" s="1">
         <v>2.1039867000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>12.350985</v>
       </c>
@@ -1441,28 +1225,22 @@
         <v>1.3566335</v>
       </c>
       <c r="C37" s="1">
-        <v>0.18054450999999999</v>
+        <v>427.84811000000002</v>
       </c>
       <c r="D37" s="1">
-        <v>356.11257999999998</v>
+        <v>12.520651000000001</v>
       </c>
       <c r="E37" s="1">
-        <v>427.84811000000002</v>
+        <v>12.165895000000001</v>
       </c>
       <c r="F37" s="1">
-        <v>12.520651000000001</v>
+        <v>2.3540268000000002</v>
       </c>
       <c r="G37" s="1">
-        <v>12.165895000000001</v>
-      </c>
-      <c r="H37" s="1">
-        <v>2.3540268000000002</v>
-      </c>
-      <c r="I37" s="1">
         <v>2.1215131</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>13.141724999999999</v>
       </c>
@@ -1470,28 +1248,22 @@
         <v>1.3238114000000001</v>
       </c>
       <c r="C38" s="1">
-        <v>0.14510565</v>
+        <v>434.17721999999998</v>
       </c>
       <c r="D38" s="1">
-        <v>357.84903000000003</v>
+        <v>13.352537</v>
       </c>
       <c r="E38" s="1">
-        <v>434.17721999999998</v>
+        <v>12.911747</v>
       </c>
       <c r="F38" s="1">
-        <v>13.352537</v>
+        <v>2.3781590000000001</v>
       </c>
       <c r="G38" s="1">
-        <v>12.911747</v>
-      </c>
-      <c r="H38" s="1">
-        <v>2.3781590000000001</v>
-      </c>
-      <c r="I38" s="1">
         <v>2.1118803000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>13.929226</v>
       </c>
@@ -1499,28 +1271,22 @@
         <v>1.2702221</v>
       </c>
       <c r="C39" s="1">
-        <v>0.11610263</v>
+        <v>440.50632000000002</v>
       </c>
       <c r="D39" s="1">
-        <v>359.60424999999998</v>
+        <v>14.146034</v>
       </c>
       <c r="E39" s="1">
-        <v>440.50632000000002</v>
+        <v>13.692708</v>
       </c>
       <c r="F39" s="1">
-        <v>14.146034</v>
+        <v>2.3276954000000001</v>
       </c>
       <c r="G39" s="1">
-        <v>13.692708</v>
-      </c>
-      <c r="H39" s="1">
-        <v>2.3276954000000001</v>
-      </c>
-      <c r="I39" s="1">
         <v>2.0625577000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>14.722943000000001</v>
       </c>
@@ -1528,28 +1294,22 @@
         <v>1.2301648000000001</v>
       </c>
       <c r="C40" s="1">
-        <v>0.13424593000000001</v>
+        <v>446.83544999999998</v>
       </c>
       <c r="D40" s="1">
-        <v>361.32339000000002</v>
+        <v>14.924105000000001</v>
       </c>
       <c r="E40" s="1">
-        <v>446.83544999999998</v>
+        <v>14.503494999999999</v>
       </c>
       <c r="F40" s="1">
-        <v>14.924105000000001</v>
+        <v>2.3872232000000002</v>
       </c>
       <c r="G40" s="1">
-        <v>14.503494999999999</v>
-      </c>
-      <c r="H40" s="1">
-        <v>2.3872232000000002</v>
-      </c>
-      <c r="I40" s="1">
         <v>2.1420876999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>15.526217000000001</v>
       </c>
@@ -1557,28 +1317,22 @@
         <v>1.1818436000000001</v>
       </c>
       <c r="C41" s="1">
-        <v>0.13468595</v>
+        <v>453.16455000000002</v>
       </c>
       <c r="D41" s="1">
-        <v>362.98703</v>
+        <v>15.782482</v>
       </c>
       <c r="E41" s="1">
-        <v>453.16455000000002</v>
+        <v>15.246655000000001</v>
       </c>
       <c r="F41" s="1">
-        <v>15.782482</v>
+        <v>2.3691099000000002</v>
       </c>
       <c r="G41" s="1">
-        <v>15.246655000000001</v>
-      </c>
-      <c r="H41" s="1">
-        <v>2.3691099000000002</v>
-      </c>
-      <c r="I41" s="1">
         <v>2.1091758999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>16.332428</v>
       </c>
@@ -1586,28 +1340,22 @@
         <v>1.1757428999999999</v>
       </c>
       <c r="C42" s="1">
-        <v>0.19271110999999999</v>
+        <v>459.49367999999998</v>
       </c>
       <c r="D42" s="1">
-        <v>364.63360999999998</v>
+        <v>16.590959999999999</v>
       </c>
       <c r="E42" s="1">
-        <v>459.49367999999998</v>
+        <v>16.050391999999999</v>
       </c>
       <c r="F42" s="1">
-        <v>16.590959999999999</v>
+        <v>2.3437412000000002</v>
       </c>
       <c r="G42" s="1">
-        <v>16.050391999999999</v>
-      </c>
-      <c r="H42" s="1">
-        <v>2.3437412000000002</v>
-      </c>
-      <c r="I42" s="1">
         <v>2.0492691999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>17.140803999999999</v>
       </c>
@@ -1615,28 +1363,22 @@
         <v>1.1096963</v>
       </c>
       <c r="C43" s="1">
-        <v>0.11879641000000001</v>
+        <v>465.82278000000002</v>
       </c>
       <c r="D43" s="1">
-        <v>366.26760999999999</v>
+        <v>17.378105000000001</v>
       </c>
       <c r="E43" s="1">
-        <v>465.82278000000002</v>
+        <v>16.881929</v>
       </c>
       <c r="F43" s="1">
-        <v>17.378105000000001</v>
+        <v>2.3010318000000001</v>
       </c>
       <c r="G43" s="1">
-        <v>16.881929</v>
-      </c>
-      <c r="H43" s="1">
-        <v>2.3010318000000001</v>
-      </c>
-      <c r="I43" s="1">
         <v>2.0399489000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>17.941739999999999</v>
       </c>
@@ -1644,28 +1386,22 @@
         <v>1.0896790999999999</v>
       </c>
       <c r="C44" s="1">
-        <v>0.14551265999999999</v>
+        <v>472.15188999999998</v>
       </c>
       <c r="D44" s="1">
-        <v>367.94481999999999</v>
+        <v>18.218031</v>
       </c>
       <c r="E44" s="1">
-        <v>472.15188999999998</v>
+        <v>17.640331</v>
       </c>
       <c r="F44" s="1">
-        <v>18.218031</v>
+        <v>2.2769493999999999</v>
       </c>
       <c r="G44" s="1">
-        <v>17.640331</v>
-      </c>
-      <c r="H44" s="1">
-        <v>2.2769493999999999</v>
-      </c>
-      <c r="I44" s="1">
         <v>2.0271845000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>18.757829999999998</v>
       </c>
@@ -1673,28 +1409,22 @@
         <v>1.0560913000000001</v>
       </c>
       <c r="C45" s="1">
-        <v>0.11999482</v>
+        <v>478.48102</v>
       </c>
       <c r="D45" s="1">
-        <v>369.53402999999997</v>
+        <v>19.017536</v>
       </c>
       <c r="E45" s="1">
-        <v>478.48102</v>
+        <v>18.474513999999999</v>
       </c>
       <c r="F45" s="1">
-        <v>19.017536</v>
+        <v>2.2776494</v>
       </c>
       <c r="G45" s="1">
-        <v>18.474513999999999</v>
-      </c>
-      <c r="H45" s="1">
-        <v>2.2776494</v>
-      </c>
-      <c r="I45" s="1">
         <v>2.0283875</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>19.570049000000001</v>
       </c>
@@ -1702,28 +1432,22 @@
         <v>1.0240334</v>
       </c>
       <c r="C46" s="1">
-        <v>9.0162045999999996E-2</v>
+        <v>484.81011999999998</v>
       </c>
       <c r="D46" s="1">
-        <v>371.14569</v>
+        <v>19.864487</v>
       </c>
       <c r="E46" s="1">
-        <v>484.81011999999998</v>
+        <v>19.248843999999998</v>
       </c>
       <c r="F46" s="1">
-        <v>19.864487</v>
+        <v>2.3117728</v>
       </c>
       <c r="G46" s="1">
-        <v>19.248843999999998</v>
-      </c>
-      <c r="H46" s="1">
-        <v>2.3117728</v>
-      </c>
-      <c r="I46" s="1">
         <v>2.0658387999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>20.387089</v>
       </c>
@@ -1731,28 +1455,22 @@
         <v>1.0153337</v>
       </c>
       <c r="C47" s="1">
-        <v>0.13769507</v>
+        <v>491.13925</v>
       </c>
       <c r="D47" s="1">
-        <v>372.72937000000002</v>
+        <v>20.720694000000002</v>
       </c>
       <c r="E47" s="1">
-        <v>491.13925</v>
+        <v>20.023154999999999</v>
       </c>
       <c r="F47" s="1">
-        <v>20.720694000000002</v>
+        <v>2.2961493000000002</v>
       </c>
       <c r="G47" s="1">
-        <v>20.023154999999999</v>
-      </c>
-      <c r="H47" s="1">
-        <v>2.2961493000000002</v>
-      </c>
-      <c r="I47" s="1">
         <v>2.0281432000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>21.198917000000002</v>
       </c>
@@ -1760,28 +1478,22 @@
         <v>0.97981315999999996</v>
       </c>
       <c r="C48" s="1">
-        <v>0.10032094</v>
+        <v>497.46834999999999</v>
       </c>
       <c r="D48" s="1">
-        <v>374.34332000000001</v>
+        <v>21.521401999999998</v>
       </c>
       <c r="E48" s="1">
-        <v>497.46834999999999</v>
+        <v>20.847116</v>
       </c>
       <c r="F48" s="1">
-        <v>21.521401999999998</v>
+        <v>2.3129778000000001</v>
       </c>
       <c r="G48" s="1">
-        <v>20.847116</v>
-      </c>
-      <c r="H48" s="1">
-        <v>2.3129778000000001</v>
-      </c>
-      <c r="I48" s="1">
         <v>2.066983</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>22.007933000000001</v>
       </c>
@@ -1789,28 +1501,22 @@
         <v>0.94907534000000005</v>
       </c>
       <c r="C49" s="1">
-        <v>0.1157991</v>
+        <v>503.79745000000003</v>
       </c>
       <c r="D49" s="1">
-        <v>375.97359999999998</v>
+        <v>22.327034000000001</v>
       </c>
       <c r="E49" s="1">
-        <v>503.79745000000003</v>
+        <v>21.659821000000001</v>
       </c>
       <c r="F49" s="1">
-        <v>22.327034000000001</v>
+        <v>2.2892833000000001</v>
       </c>
       <c r="G49" s="1">
-        <v>21.659821000000001</v>
-      </c>
-      <c r="H49" s="1">
-        <v>2.2892833000000001</v>
-      </c>
-      <c r="I49" s="1">
         <v>2.045938</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>22.823996000000001</v>
       </c>
@@ -1818,28 +1524,22 @@
         <v>0.92917395000000003</v>
       </c>
       <c r="C50" s="1">
-        <v>9.8905778999999999E-2</v>
+        <v>510.12659000000002</v>
       </c>
       <c r="D50" s="1">
-        <v>377.56295999999998</v>
+        <v>23.175453000000001</v>
       </c>
       <c r="E50" s="1">
-        <v>510.12659000000002</v>
+        <v>22.44059</v>
       </c>
       <c r="F50" s="1">
-        <v>23.175453000000001</v>
+        <v>2.2495536999999999</v>
       </c>
       <c r="G50" s="1">
-        <v>22.44059</v>
-      </c>
-      <c r="H50" s="1">
-        <v>2.2495536999999999</v>
-      </c>
-      <c r="I50" s="1">
         <v>1.9953978000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>23.637135000000001</v>
       </c>
@@ -1847,28 +1547,22 @@
         <v>0.91878300999999996</v>
       </c>
       <c r="C51" s="1">
-        <v>7.8379497000000006E-2</v>
+        <v>516.45569</v>
       </c>
       <c r="D51" s="1">
-        <v>379.16931</v>
+        <v>24.005344000000001</v>
       </c>
       <c r="E51" s="1">
-        <v>516.45569</v>
+        <v>23.235448999999999</v>
       </c>
       <c r="F51" s="1">
-        <v>24.005344000000001</v>
+        <v>2.2700281000000002</v>
       </c>
       <c r="G51" s="1">
-        <v>23.235448999999999</v>
-      </c>
-      <c r="H51" s="1">
-        <v>2.2700281000000002</v>
-      </c>
-      <c r="I51" s="1">
         <v>2.0083799</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>24.448098999999999</v>
       </c>
@@ -1876,28 +1570,22 @@
         <v>0.91100835999999996</v>
       </c>
       <c r="C52" s="1">
-        <v>9.6605889E-2</v>
+        <v>522.78479000000004</v>
       </c>
       <c r="D52" s="1">
-        <v>380.78827000000001</v>
+        <v>24.825838000000001</v>
       </c>
       <c r="E52" s="1">
-        <v>522.78479000000004</v>
+        <v>24.036020000000001</v>
       </c>
       <c r="F52" s="1">
-        <v>24.825838000000001</v>
+        <v>2.2840091999999999</v>
       </c>
       <c r="G52" s="1">
-        <v>24.036020000000001</v>
-      </c>
-      <c r="H52" s="1">
-        <v>2.2840091999999999</v>
-      </c>
-      <c r="I52" s="1">
         <v>2.0251420000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>25.255575</v>
       </c>
@@ -1905,28 +1593,22 @@
         <v>0.88468647</v>
       </c>
       <c r="C53" s="1">
-        <v>5.9167400000000002E-2</v>
+        <v>529.11395000000005</v>
       </c>
       <c r="D53" s="1">
-        <v>382.42748999999998</v>
+        <v>25.620128999999999</v>
       </c>
       <c r="E53" s="1">
-        <v>529.11395000000005</v>
+        <v>24.857882</v>
       </c>
       <c r="F53" s="1">
-        <v>25.620128999999999</v>
+        <v>2.2964159999999998</v>
       </c>
       <c r="G53" s="1">
-        <v>24.857882</v>
-      </c>
-      <c r="H53" s="1">
-        <v>2.2964159999999998</v>
-      </c>
-      <c r="I53" s="1">
         <v>2.0335549999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>26.063147000000001</v>
       </c>
@@ -1934,28 +1616,22 @@
         <v>0.86158729000000001</v>
       </c>
       <c r="C54" s="1">
-        <v>0.10526272</v>
+        <v>535.44304999999997</v>
       </c>
       <c r="D54" s="1">
-        <v>384.06616000000002</v>
+        <v>26.458985999999999</v>
       </c>
       <c r="E54" s="1">
-        <v>535.44304999999997</v>
+        <v>25.631322999999998</v>
       </c>
       <c r="F54" s="1">
-        <v>26.458985999999999</v>
+        <v>2.2240101999999999</v>
       </c>
       <c r="G54" s="1">
-        <v>25.631322999999998</v>
-      </c>
-      <c r="H54" s="1">
-        <v>2.2240101999999999</v>
-      </c>
-      <c r="I54" s="1">
         <v>1.9863888999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>26.869406000000001</v>
       </c>
@@ -1963,28 +1639,22 @@
         <v>0.85107480999999996</v>
       </c>
       <c r="C55" s="1">
-        <v>6.0117133000000003E-2</v>
+        <v>541.77215999999999</v>
       </c>
       <c r="D55" s="1">
-        <v>385.71246000000002</v>
+        <v>27.255807999999998</v>
       </c>
       <c r="E55" s="1">
-        <v>541.77215999999999</v>
+        <v>26.447873999999999</v>
       </c>
       <c r="F55" s="1">
-        <v>27.255807999999998</v>
+        <v>2.2650367999999999</v>
       </c>
       <c r="G55" s="1">
-        <v>26.447873999999999</v>
-      </c>
-      <c r="H55" s="1">
-        <v>2.2650367999999999</v>
-      </c>
-      <c r="I55" s="1">
         <v>2.0065485999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>27.678163999999999</v>
       </c>
@@ -1992,28 +1662,22 @@
         <v>0.83907997999999995</v>
       </c>
       <c r="C56" s="1">
-        <v>9.7365804E-2</v>
+        <v>548.10126000000002</v>
       </c>
       <c r="D56" s="1">
-        <v>387.34426999999999</v>
+        <v>28.064131</v>
       </c>
       <c r="E56" s="1">
-        <v>548.10126000000002</v>
+        <v>27.257107000000001</v>
       </c>
       <c r="F56" s="1">
-        <v>28.064131</v>
+        <v>2.2132466000000002</v>
       </c>
       <c r="G56" s="1">
-        <v>27.257107000000001</v>
-      </c>
-      <c r="H56" s="1">
-        <v>2.2132466000000002</v>
-      </c>
-      <c r="I56" s="1">
         <v>1.9768007999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>28.48358</v>
       </c>
@@ -2021,28 +1685,22 @@
         <v>0.82168191999999995</v>
       </c>
       <c r="C57" s="1">
-        <v>9.1928624E-2</v>
+        <v>554.43035999999995</v>
       </c>
       <c r="D57" s="1">
-        <v>388.99545000000001</v>
+        <v>28.899597</v>
       </c>
       <c r="E57" s="1">
-        <v>554.43035999999995</v>
+        <v>28.029744999999998</v>
       </c>
       <c r="F57" s="1">
-        <v>28.899597</v>
+        <v>2.1961756000000001</v>
       </c>
       <c r="G57" s="1">
-        <v>28.029744999999998</v>
-      </c>
-      <c r="H57" s="1">
-        <v>2.1961756000000001</v>
-      </c>
-      <c r="I57" s="1">
         <v>1.964669</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>29.285719</v>
       </c>
@@ -2050,28 +1708,22 @@
         <v>0.81182449999999995</v>
       </c>
       <c r="C58" s="1">
-        <v>6.9946281999999999E-2</v>
+        <v>560.75951999999995</v>
       </c>
       <c r="D58" s="1">
-        <v>390.66568000000001</v>
+        <v>29.718008000000001</v>
       </c>
       <c r="E58" s="1">
-        <v>560.75951999999995</v>
+        <v>28.814131</v>
       </c>
       <c r="F58" s="1">
-        <v>29.718008000000001</v>
+        <v>2.2257764</v>
       </c>
       <c r="G58" s="1">
-        <v>28.814131</v>
-      </c>
-      <c r="H58" s="1">
-        <v>2.2257764</v>
-      </c>
-      <c r="I58" s="1">
         <v>1.9846349000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>30.082004999999999</v>
       </c>
@@ -2079,28 +1731,22 @@
         <v>0.79835891999999997</v>
       </c>
       <c r="C59" s="1">
-        <v>4.0003877E-2</v>
+        <v>567.08861999999999</v>
       </c>
       <c r="D59" s="1">
-        <v>392.36989999999997</v>
+        <v>30.507743999999999</v>
       </c>
       <c r="E59" s="1">
-        <v>567.08861999999999</v>
+        <v>29.617564999999999</v>
       </c>
       <c r="F59" s="1">
-        <v>30.507743999999999</v>
+        <v>2.2300230999999999</v>
       </c>
       <c r="G59" s="1">
-        <v>29.617564999999999</v>
-      </c>
-      <c r="H59" s="1">
-        <v>2.2300230999999999</v>
-      </c>
-      <c r="I59" s="1">
         <v>1.9787359</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>30.879221000000001</v>
       </c>
@@ -2108,28 +1754,22 @@
         <v>0.78214877999999999</v>
       </c>
       <c r="C60" s="1">
-        <v>5.6926310000000001E-2</v>
+        <v>573.41772000000003</v>
       </c>
       <c r="D60" s="1">
-        <v>394.06873000000002</v>
+        <v>31.329597</v>
       </c>
       <c r="E60" s="1">
-        <v>573.41772000000003</v>
+        <v>30.387900999999999</v>
       </c>
       <c r="F60" s="1">
-        <v>31.329597</v>
+        <v>2.2642783999999998</v>
       </c>
       <c r="G60" s="1">
-        <v>30.387900999999999</v>
-      </c>
-      <c r="H60" s="1">
-        <v>2.2642783999999998</v>
-      </c>
-      <c r="I60" s="1">
         <v>2.0103395000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>31.674624999999999</v>
       </c>
@@ -2137,28 +1777,22 @@
         <v>0.76700318000000001</v>
       </c>
       <c r="C61" s="1">
-        <v>6.3085862000000006E-2</v>
+        <v>579.74683000000005</v>
       </c>
       <c r="D61" s="1">
-        <v>395.77805000000001</v>
+        <v>32.138336000000002</v>
       </c>
       <c r="E61" s="1">
-        <v>579.74683000000005</v>
+        <v>31.168758</v>
       </c>
       <c r="F61" s="1">
-        <v>32.138336000000002</v>
+        <v>2.1508392999999999</v>
       </c>
       <c r="G61" s="1">
-        <v>31.168758</v>
-      </c>
-      <c r="H61" s="1">
-        <v>2.1508392999999999</v>
-      </c>
-      <c r="I61" s="1">
         <v>1.9151924</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>32.462662000000002</v>
       </c>
@@ -2166,28 +1800,22 @@
         <v>0.75403648999999995</v>
       </c>
       <c r="C62" s="1">
-        <v>1.8382725999999999E-2</v>
+        <v>586.07592999999997</v>
       </c>
       <c r="D62" s="1">
-        <v>397.53017999999997</v>
+        <v>32.934868000000002</v>
       </c>
       <c r="E62" s="1">
-        <v>586.07592999999997</v>
+        <v>31.947527000000001</v>
       </c>
       <c r="F62" s="1">
-        <v>32.934868000000002</v>
+        <v>2.1765232000000001</v>
       </c>
       <c r="G62" s="1">
-        <v>31.947527000000001</v>
-      </c>
-      <c r="H62" s="1">
-        <v>2.1765232000000001</v>
-      </c>
-      <c r="I62" s="1">
         <v>1.9509989000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>33.254181000000003</v>
       </c>
@@ -2195,28 +1823,22 @@
         <v>0.75168341000000005</v>
       </c>
       <c r="C63" s="1">
-        <v>3.8608689000000002E-2</v>
+        <v>592.40508999999997</v>
       </c>
       <c r="D63" s="1">
-        <v>399.26208000000003</v>
+        <v>33.755851999999997</v>
       </c>
       <c r="E63" s="1">
-        <v>592.40508999999997</v>
+        <v>32.706904999999999</v>
       </c>
       <c r="F63" s="1">
-        <v>33.755851999999997</v>
+        <v>2.1898610999999999</v>
       </c>
       <c r="G63" s="1">
-        <v>32.706904999999999</v>
-      </c>
-      <c r="H63" s="1">
-        <v>2.1898610999999999</v>
-      </c>
-      <c r="I63" s="1">
         <v>1.9523752000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>34.038330000000002</v>
       </c>
@@ -2224,28 +1846,22 @@
         <v>0.73663491000000003</v>
       </c>
       <c r="C64" s="1">
-        <v>6.8239056000000006E-2</v>
+        <v>598.73419000000001</v>
       </c>
       <c r="D64" s="1">
-        <v>401.03680000000003</v>
+        <v>34.565444999999997</v>
       </c>
       <c r="E64" s="1">
-        <v>598.73419000000001</v>
+        <v>33.463298999999999</v>
       </c>
       <c r="F64" s="1">
-        <v>34.565444999999997</v>
+        <v>2.2007227</v>
       </c>
       <c r="G64" s="1">
-        <v>33.463298999999999</v>
-      </c>
-      <c r="H64" s="1">
-        <v>2.2007227</v>
-      </c>
-      <c r="I64" s="1">
         <v>1.9656891000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>34.821434000000004</v>
       </c>
@@ -2253,28 +1869,22 @@
         <v>0.73090655000000004</v>
       </c>
       <c r="C65" s="1">
-        <v>6.2995336999999998E-2</v>
+        <v>605.06329000000005</v>
       </c>
       <c r="D65" s="1">
-        <v>402.81760000000003</v>
+        <v>35.339989000000003</v>
       </c>
       <c r="E65" s="1">
-        <v>605.06329000000005</v>
+        <v>34.255737000000003</v>
       </c>
       <c r="F65" s="1">
-        <v>35.339989000000003</v>
+        <v>2.0812062999999998</v>
       </c>
       <c r="G65" s="1">
-        <v>34.255737000000003</v>
-      </c>
-      <c r="H65" s="1">
-        <v>2.0812062999999998</v>
-      </c>
-      <c r="I65" s="1">
         <v>1.860123</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>35.595954999999996</v>
       </c>
@@ -2282,28 +1892,22 @@
         <v>0.71562278000000001</v>
       </c>
       <c r="C66" s="1">
-        <v>2.9919086000000001E-2</v>
+        <v>611.39239999999995</v>
       </c>
       <c r="D66" s="1">
-        <v>404.64821999999998</v>
+        <v>36.089953999999999</v>
       </c>
       <c r="E66" s="1">
-        <v>611.39239999999995</v>
+        <v>35.057048999999999</v>
       </c>
       <c r="F66" s="1">
-        <v>36.089953999999999</v>
+        <v>2.1682332</v>
       </c>
       <c r="G66" s="1">
-        <v>35.057048999999999</v>
-      </c>
-      <c r="H66" s="1">
-        <v>2.1682332</v>
-      </c>
-      <c r="I66" s="1">
         <v>1.9227192</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>36.371861000000003</v>
       </c>
@@ -2311,28 +1915,22 @@
         <v>0.72298205000000004</v>
       </c>
       <c r="C67" s="1">
-        <v>8.3936140000000006E-2</v>
+        <v>617.72149999999999</v>
       </c>
       <c r="D67" s="1">
-        <v>406.47082999999998</v>
+        <v>36.885455999999998</v>
       </c>
       <c r="E67" s="1">
-        <v>617.72149999999999</v>
+        <v>35.811577</v>
       </c>
       <c r="F67" s="1">
-        <v>36.885455999999998</v>
+        <v>2.1670356000000002</v>
       </c>
       <c r="G67" s="1">
-        <v>35.811577</v>
-      </c>
-      <c r="H67" s="1">
-        <v>2.1670356000000002</v>
-      </c>
-      <c r="I67" s="1">
         <v>1.9195545000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>37.142375999999999</v>
       </c>
@@ -2340,28 +1938,22 @@
         <v>0.70196289000000001</v>
       </c>
       <c r="C68" s="1">
-        <v>2.1597253E-2</v>
+        <v>624.05065999999999</v>
       </c>
       <c r="D68" s="1">
-        <v>408.32470999999998</v>
+        <v>37.678714999999997</v>
       </c>
       <c r="E68" s="1">
-        <v>624.05065999999999</v>
+        <v>36.557277999999997</v>
       </c>
       <c r="F68" s="1">
-        <v>37.678714999999997</v>
+        <v>2.1281259000000001</v>
       </c>
       <c r="G68" s="1">
-        <v>36.557277999999997</v>
-      </c>
-      <c r="H68" s="1">
-        <v>2.1281259000000001</v>
-      </c>
-      <c r="I68" s="1">
         <v>1.8943460999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>37.911045000000001</v>
       </c>
@@ -2369,28 +1961,22 @@
         <v>0.69111674999999995</v>
       </c>
       <c r="C69" s="1">
-        <v>1.5703600000000002E-2</v>
+        <v>630.37976000000003</v>
       </c>
       <c r="D69" s="1">
-        <v>410.18932999999998</v>
+        <v>38.479900000000001</v>
       </c>
       <c r="E69" s="1">
-        <v>630.37976000000003</v>
+        <v>37.290478</v>
       </c>
       <c r="F69" s="1">
-        <v>38.479900000000001</v>
+        <v>2.1509347000000001</v>
       </c>
       <c r="G69" s="1">
-        <v>37.290478</v>
-      </c>
-      <c r="H69" s="1">
-        <v>2.1509347000000001</v>
-      </c>
-      <c r="I69" s="1">
         <v>1.9108996</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>38.672275999999997</v>
       </c>
@@ -2398,28 +1984,22 @@
         <v>0.68877745000000001</v>
       </c>
       <c r="C70" s="1">
-        <v>5.6048460000000001E-2</v>
+        <v>636.70885999999996</v>
       </c>
       <c r="D70" s="1">
-        <v>412.09717000000001</v>
+        <v>39.237727999999997</v>
       </c>
       <c r="E70" s="1">
-        <v>636.70885999999996</v>
+        <v>38.055419999999998</v>
       </c>
       <c r="F70" s="1">
-        <v>39.237727999999997</v>
+        <v>2.1365509</v>
       </c>
       <c r="G70" s="1">
-        <v>38.055419999999998</v>
-      </c>
-      <c r="H70" s="1">
-        <v>2.1365509</v>
-      </c>
-      <c r="I70" s="1">
         <v>1.9061341999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>39.431137</v>
       </c>
@@ -2427,28 +2007,22 @@
         <v>0.68405724000000001</v>
       </c>
       <c r="C71" s="1">
-        <v>-6.3795535999999998E-3</v>
+        <v>643.03796</v>
       </c>
       <c r="D71" s="1">
-        <v>414.01873999999998</v>
+        <v>40.012805999999998</v>
       </c>
       <c r="E71" s="1">
-        <v>643.03796</v>
+        <v>38.796588999999997</v>
       </c>
       <c r="F71" s="1">
-        <v>40.012805999999998</v>
+        <v>2.1401252999999998</v>
       </c>
       <c r="G71" s="1">
-        <v>38.796588999999997</v>
-      </c>
-      <c r="H71" s="1">
-        <v>2.1401252999999998</v>
-      </c>
-      <c r="I71" s="1">
         <v>1.891311</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>40.184699999999999</v>
       </c>
@@ -2456,28 +2030,22 @@
         <v>0.67477279999999995</v>
       </c>
       <c r="C72" s="1">
-        <v>5.2706546999999999E-2</v>
+        <v>649.36707000000001</v>
       </c>
       <c r="D72" s="1">
-        <v>415.97109999999998</v>
+        <v>40.759911000000002</v>
       </c>
       <c r="E72" s="1">
-        <v>649.36707000000001</v>
+        <v>39.557198</v>
       </c>
       <c r="F72" s="1">
-        <v>40.759911000000002</v>
+        <v>2.1722204999999999</v>
       </c>
       <c r="G72" s="1">
-        <v>39.557198</v>
-      </c>
-      <c r="H72" s="1">
-        <v>2.1722204999999999</v>
-      </c>
-      <c r="I72" s="1">
         <v>1.9272469999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>40.937992000000001</v>
       </c>
@@ -2485,28 +2053,22 @@
         <v>0.66115338000000001</v>
       </c>
       <c r="C73" s="1">
-        <v>2.9512067999999999E-2</v>
+        <v>655.69623000000001</v>
       </c>
       <c r="D73" s="1">
-        <v>417.92505</v>
+        <v>41.573462999999997</v>
       </c>
       <c r="E73" s="1">
-        <v>655.69623000000001</v>
+        <v>40.244746999999997</v>
       </c>
       <c r="F73" s="1">
-        <v>41.573462999999997</v>
+        <v>2.1742194000000001</v>
       </c>
       <c r="G73" s="1">
-        <v>40.244746999999997</v>
-      </c>
-      <c r="H73" s="1">
-        <v>2.1742194000000001</v>
-      </c>
-      <c r="I73" s="1">
         <v>1.9359388</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>41.681010999999998</v>
       </c>
@@ -2514,28 +2076,22 @@
         <v>0.65015155000000002</v>
       </c>
       <c r="C74" s="1">
-        <v>7.0203119000000003E-3</v>
+        <v>662.02533000000005</v>
       </c>
       <c r="D74" s="1">
-        <v>419.93862999999999</v>
+        <v>42.292385000000003</v>
       </c>
       <c r="E74" s="1">
-        <v>662.02533000000005</v>
+        <v>41.014060999999998</v>
       </c>
       <c r="F74" s="1">
-        <v>42.292385000000003</v>
+        <v>2.1411511999999999</v>
       </c>
       <c r="G74" s="1">
-        <v>41.014060999999998</v>
-      </c>
-      <c r="H74" s="1">
-        <v>2.1411511999999999</v>
-      </c>
-      <c r="I74" s="1">
         <v>1.9092986999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>42.424221000000003</v>
       </c>
@@ -2543,28 +2099,22 @@
         <v>0.65401608</v>
       </c>
       <c r="C75" s="1">
-        <v>-1.3033384999999999E-4</v>
+        <v>668.35442999999998</v>
       </c>
       <c r="D75" s="1">
-        <v>421.95114000000001</v>
+        <v>43.036079000000001</v>
       </c>
       <c r="E75" s="1">
-        <v>668.35442999999998</v>
+        <v>41.756740999999998</v>
       </c>
       <c r="F75" s="1">
-        <v>43.036079000000001</v>
+        <v>2.1143599000000002</v>
       </c>
       <c r="G75" s="1">
-        <v>41.756740999999998</v>
-      </c>
-      <c r="H75" s="1">
-        <v>2.1143599000000002</v>
-      </c>
-      <c r="I75" s="1">
         <v>1.8770591000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43.160693999999999</v>
       </c>
@@ -2572,28 +2122,22 @@
         <v>0.64330869999999996</v>
       </c>
       <c r="C76" s="1">
-        <v>3.3431228E-2</v>
+        <v>674.68353000000002</v>
       </c>
       <c r="D76" s="1">
-        <v>424.00274999999999</v>
+        <v>43.818851000000002</v>
       </c>
       <c r="E76" s="1">
-        <v>674.68353000000002</v>
+        <v>42.442703000000002</v>
       </c>
       <c r="F76" s="1">
-        <v>43.818851000000002</v>
+        <v>2.0844238000000002</v>
       </c>
       <c r="G76" s="1">
-        <v>42.442703000000002</v>
-      </c>
-      <c r="H76" s="1">
-        <v>2.0844238000000002</v>
-      </c>
-      <c r="I76" s="1">
         <v>1.8526142999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43.886284000000003</v>
       </c>
@@ -2601,28 +2145,22 @@
         <v>0.63395751</v>
       </c>
       <c r="C77" s="1">
-        <v>2.4451798E-2</v>
+        <v>681.01262999999994</v>
       </c>
       <c r="D77" s="1">
-        <v>426.11757999999998</v>
+        <v>44.480808000000003</v>
       </c>
       <c r="E77" s="1">
-        <v>681.01262999999994</v>
+        <v>43.237709000000002</v>
       </c>
       <c r="F77" s="1">
-        <v>44.480808000000003</v>
+        <v>2.1464390999999998</v>
       </c>
       <c r="G77" s="1">
-        <v>43.237709000000002</v>
-      </c>
-      <c r="H77" s="1">
-        <v>2.1464390999999998</v>
-      </c>
-      <c r="I77" s="1">
         <v>1.9076887</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44.616061999999999</v>
       </c>
@@ -2630,28 +2168,22 @@
         <v>0.62282592000000003</v>
       </c>
       <c r="C78" s="1">
-        <v>1.4460974999999999E-2</v>
+        <v>687.34180000000003</v>
       </c>
       <c r="D78" s="1">
-        <v>428.20807000000002</v>
+        <v>45.272754999999997</v>
       </c>
       <c r="E78" s="1">
-        <v>687.34180000000003</v>
+        <v>43.899673</v>
       </c>
       <c r="F78" s="1">
-        <v>45.272754999999997</v>
+        <v>2.1101911000000002</v>
       </c>
       <c r="G78" s="1">
-        <v>43.899673</v>
-      </c>
-      <c r="H78" s="1">
-        <v>2.1101911000000002</v>
-      </c>
-      <c r="I78" s="1">
         <v>1.8724778</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45.336395000000003</v>
       </c>
@@ -2659,28 +2191,22 @@
         <v>0.62137109000000001</v>
       </c>
       <c r="C79" s="1">
-        <v>1.3353947999999999E-2</v>
+        <v>693.67089999999996</v>
       </c>
       <c r="D79" s="1">
-        <v>430.35342000000003</v>
+        <v>46.010779999999997</v>
       </c>
       <c r="E79" s="1">
-        <v>693.67089999999996</v>
+        <v>44.600700000000003</v>
       </c>
       <c r="F79" s="1">
-        <v>46.010779999999997</v>
+        <v>2.0717846999999998</v>
       </c>
       <c r="G79" s="1">
-        <v>44.600700000000003</v>
-      </c>
-      <c r="H79" s="1">
-        <v>2.0717846999999998</v>
-      </c>
-      <c r="I79" s="1">
         <v>1.8431245000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>46.052238000000003</v>
       </c>
@@ -2688,24 +2214,18 @@
         <v>0.61225677000000001</v>
       </c>
       <c r="C80" s="1">
-        <v>3.1440890999999999E-2</v>
+        <v>700</v>
       </c>
       <c r="D80" s="1">
-        <v>432.52487000000002</v>
+        <v>46.714503999999998</v>
       </c>
       <c r="E80" s="1">
-        <v>700</v>
+        <v>45.329765000000002</v>
       </c>
       <c r="F80" s="1">
-        <v>46.714503999999998</v>
+        <v>2.1084665999999999</v>
       </c>
       <c r="G80" s="1">
-        <v>45.329765000000002</v>
-      </c>
-      <c r="H80" s="1">
-        <v>2.1084665999999999</v>
-      </c>
-      <c r="I80" s="1">
         <v>1.8735009</v>
       </c>
     </row>

</xml_diff>